<commit_message>
Célula B3 mesclada com C3
</commit_message>
<xml_diff>
--- a/FORM-TROCAS.xlsx
+++ b/FORM-TROCAS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esc_102\Documents\INTEGRACOES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esc_102\Documents\INTEGRACOES\sistema_troca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94F7DCD-0420-440F-A7B4-CB5F128E11AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E428C750-9E17-43E7-B145-3296FA901F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -140,11 +140,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -164,8 +190,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +504,7 @@
   <dimension ref="A2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,19 +516,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,6 +727,9 @@
       <c r="C35" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: Inserção da DATA nas células D3 e D4
</commit_message>
<xml_diff>
--- a/FORM-TROCAS.xlsx
+++ b/FORM-TROCAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esc_102\Documents\INTEGRACOES\sistema_troca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esc_106\Documents\sistema_troca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600A16F2-88D3-4DF7-9D7A-7FAADB15D4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544E86DE-B5DA-498A-AA34-AF2D44AE0683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>FORNECEDOR</t>
   </si>
@@ -73,12 +73,15 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>DATA:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +115,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,6 +203,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +517,7 @@
   <dimension ref="A2:I305"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E305"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +541,13 @@
     <row r="3" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="C3"/>
-      <c r="D3"/>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>

</xml_diff>